<commit_message>
Added the validation summary report for PikesPeakBoces (Iteration #1).
</commit_message>
<xml_diff>
--- a/Docs/SPED/Validation Reports/Mesa51/Enrich-ETL-Data-Validation-Report-Mesa-51-Iteration-9.xlsx
+++ b/Docs/SPED/Validation Reports/Mesa51/Enrich-ETL-Data-Validation-Report-Mesa-51-Iteration-9.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="62">
   <si>
     <t>File Type</t>
   </si>
@@ -562,28 +562,10 @@
 </t>
   </si>
   <si>
-    <r>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SPLC, FA, RES, SNT and few other codes should exist in SelectList file. These codes are existed in Service file(in ServiceDefinitionCode &amp;  ServiceProviderTitleCode columns).</t>
-    </r>
+    <t xml:space="preserve">1. Some  IEPRefIDs do not exist in IEP file.
+2. Some  ServiceProvider codes do not exist in SelectLists file.  They are : MNT, SNT, RES,SSN, and DEAF. But these  existed in Service file(in ServiceProviderTitleCode column).
+3. Some ServiceDefinition codes do not exist in Selectlists file. They are: LITC, MAC, LMC, LANC, SPLC, and  FA.   But these  existed in Service file(in ServiceDefinitionCode column).
+</t>
   </si>
 </sst>
 </file>
@@ -1088,52 +1070,70 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1144,52 +1144,34 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1496,7 +1478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1823,24 +1805,24 @@
     </row>
     <row r="22" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:6" hidden="1">
-      <c r="A24" s="33"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
@@ -1850,62 +1832,58 @@
       <c r="A25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="B25" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
-      <c r="A26" s="32"/>
-      <c r="B26" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-    </row>
-    <row r="27" spans="1:6" ht="54" customHeight="1">
-      <c r="A27" s="32"/>
-      <c r="B27" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:6" ht="78" customHeight="1">
+      <c r="A27" s="42"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A31" s="35"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
@@ -2227,40 +2205,40 @@
       <c r="A55" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A56" s="32"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
+      <c r="A56" s="42"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:6" hidden="1">
-      <c r="A57" s="32"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
+      <c r="A57" s="42"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="1:6" ht="44.25" customHeight="1">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="33"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="40"/>
       <c r="C59" s="41"/>
       <c r="D59" s="41"/>
@@ -2270,78 +2248,78 @@
       <c r="A60" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1">
-      <c r="A61" s="32"/>
-      <c r="B61" s="38" t="s">
+      <c r="A61" s="42"/>
+      <c r="B61" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A62" s="32"/>
+      <c r="A62" s="42"/>
       <c r="B62" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="34" t="s">
+      <c r="B63" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
-      <c r="A64" s="32"/>
-      <c r="B64" s="34" t="s">
+      <c r="A64" s="42"/>
+      <c r="B64" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A65" s="33"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
+      <c r="A65" s="32"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A67" s="35"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A68" s="35"/>
+      <c r="A68" s="34"/>
       <c r="B68" s="26"/>
       <c r="C68" s="23"/>
       <c r="D68" s="23"/>
@@ -2663,42 +2641,42 @@
       <c r="A92" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B92" s="37" t="s">
+      <c r="B92" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1">
-      <c r="A93" s="32"/>
-      <c r="B93" s="34" t="s">
+      <c r="A93" s="42"/>
+      <c r="B93" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="33"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="33"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
+      <c r="A94" s="32"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="1:6" ht="44.25" customHeight="1">
-      <c r="A95" s="65" t="s">
+      <c r="A95" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B95" s="36" t="s">
+      <c r="B95" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="65"/>
+      <c r="A96" s="51"/>
       <c r="B96" s="40"/>
       <c r="C96" s="41"/>
       <c r="D96" s="41"/>
@@ -2708,80 +2686,80 @@
       <c r="A97" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B97" s="38" t="s">
+      <c r="B97" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C97" s="42"/>
-      <c r="D97" s="42"/>
-      <c r="E97" s="42"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="49"/>
+      <c r="E97" s="49"/>
     </row>
     <row r="98" spans="1:5" ht="15" customHeight="1">
-      <c r="A98" s="32"/>
-      <c r="B98" s="38" t="s">
+      <c r="A98" s="42"/>
+      <c r="B98" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="42"/>
-      <c r="D98" s="42"/>
-      <c r="E98" s="42"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="49"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A99" s="32"/>
+      <c r="A99" s="42"/>
       <c r="B99" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="43"/>
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
     </row>
     <row r="100" spans="1:5" ht="15" customHeight="1">
       <c r="A100" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B100" s="34" t="s">
+      <c r="B100" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C100" s="34"/>
-      <c r="D100" s="34"/>
-      <c r="E100" s="34"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
     </row>
     <row r="101" spans="1:5" ht="15" customHeight="1">
-      <c r="A101" s="32"/>
-      <c r="B101" s="34" t="s">
+      <c r="A101" s="42"/>
+      <c r="B101" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="34"/>
-      <c r="D101" s="34"/>
-      <c r="E101" s="34"/>
+      <c r="C101" s="33"/>
+      <c r="D101" s="33"/>
+      <c r="E101" s="33"/>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A102" s="33"/>
-      <c r="B102" s="34"/>
-      <c r="C102" s="34"/>
-      <c r="D102" s="34"/>
-      <c r="E102" s="34"/>
+      <c r="A102" s="32"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="33"/>
     </row>
     <row r="103" spans="1:5" ht="15" customHeight="1">
-      <c r="A103" s="35" t="s">
+      <c r="A103" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B103" s="36" t="s">
+      <c r="B103" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C103" s="37"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="37"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="36"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A104" s="35"/>
-      <c r="B104" s="38" t="s">
+      <c r="A104" s="34"/>
+      <c r="B104" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C104" s="34"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33"/>
+      <c r="E104" s="33"/>
     </row>
     <row r="105" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A105" s="35"/>
+      <c r="A105" s="34"/>
       <c r="B105" s="26"/>
       <c r="C105" s="21"/>
       <c r="D105" s="21"/>
@@ -3083,215 +3061,215 @@
       </c>
     </row>
     <row r="128" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A128" s="58" t="s">
+      <c r="A128" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B128" s="58"/>
-      <c r="C128" s="58"/>
-      <c r="D128" s="58"/>
-      <c r="E128" s="58"/>
+      <c r="B128" s="63"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
     </row>
     <row r="129" spans="1:5" ht="15.75" thickBot="1">
       <c r="A129" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B129" s="56" t="s">
+      <c r="B129" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C129" s="57"/>
-      <c r="D129" s="57"/>
-      <c r="E129" s="57"/>
+      <c r="C129" s="65"/>
+      <c r="D129" s="65"/>
+      <c r="E129" s="65"/>
     </row>
     <row r="130" spans="1:5" ht="30.75" customHeight="1" thickTop="1">
-      <c r="A130" s="52" t="s">
+      <c r="A130" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B130" s="51" t="s">
+      <c r="B130" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="34"/>
-      <c r="D130" s="34"/>
-      <c r="E130" s="34"/>
+      <c r="C130" s="33"/>
+      <c r="D130" s="33"/>
+      <c r="E130" s="33"/>
     </row>
     <row r="131" spans="1:5" ht="15" customHeight="1">
-      <c r="A131" s="53"/>
-      <c r="B131" s="51" t="s">
+      <c r="A131" s="59"/>
+      <c r="B131" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C131" s="34"/>
-      <c r="D131" s="34"/>
-      <c r="E131" s="34"/>
+      <c r="C131" s="33"/>
+      <c r="D131" s="33"/>
+      <c r="E131" s="33"/>
     </row>
     <row r="132" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A132" s="54"/>
-      <c r="B132" s="51"/>
-      <c r="C132" s="34"/>
-      <c r="D132" s="34"/>
-      <c r="E132" s="34"/>
+      <c r="A132" s="60"/>
+      <c r="B132" s="57"/>
+      <c r="C132" s="33"/>
+      <c r="D132" s="33"/>
+      <c r="E132" s="33"/>
     </row>
     <row r="133" spans="1:5" ht="44.25" customHeight="1">
-      <c r="A133" s="55" t="s">
+      <c r="A133" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B133" s="51" t="s">
+      <c r="B133" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C133" s="34"/>
-      <c r="D133" s="34"/>
-      <c r="E133" s="34"/>
+      <c r="C133" s="33"/>
+      <c r="D133" s="33"/>
+      <c r="E133" s="33"/>
     </row>
     <row r="134" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A134" s="54"/>
-      <c r="B134" s="51"/>
-      <c r="C134" s="34"/>
-      <c r="D134" s="34"/>
-      <c r="E134" s="34"/>
+      <c r="A134" s="60"/>
+      <c r="B134" s="57"/>
+      <c r="C134" s="33"/>
+      <c r="D134" s="33"/>
+      <c r="E134" s="33"/>
     </row>
     <row r="135" spans="1:5" ht="15" customHeight="1">
-      <c r="A135" s="55" t="s">
+      <c r="A135" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B135" s="51" t="s">
+      <c r="B135" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C135" s="34"/>
-      <c r="D135" s="34"/>
-      <c r="E135" s="34"/>
+      <c r="C135" s="33"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="33"/>
     </row>
     <row r="136" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A136" s="54"/>
-      <c r="B136" s="51"/>
-      <c r="C136" s="34"/>
-      <c r="D136" s="34"/>
-      <c r="E136" s="34"/>
+      <c r="A136" s="60"/>
+      <c r="B136" s="57"/>
+      <c r="C136" s="33"/>
+      <c r="D136" s="33"/>
+      <c r="E136" s="33"/>
     </row>
     <row r="137" spans="1:5" ht="15" customHeight="1">
-      <c r="A137" s="55" t="s">
+      <c r="A137" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B137" s="51" t="s">
+      <c r="B137" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C137" s="34"/>
-      <c r="D137" s="34"/>
-      <c r="E137" s="34"/>
+      <c r="C137" s="33"/>
+      <c r="D137" s="33"/>
+      <c r="E137" s="33"/>
     </row>
     <row r="138" spans="1:5" ht="15" customHeight="1">
-      <c r="A138" s="53"/>
-      <c r="B138" s="51" t="s">
+      <c r="A138" s="59"/>
+      <c r="B138" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C138" s="34"/>
-      <c r="D138" s="34"/>
-      <c r="E138" s="34"/>
+      <c r="C138" s="33"/>
+      <c r="D138" s="33"/>
+      <c r="E138" s="33"/>
     </row>
     <row r="139" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A139" s="54"/>
-      <c r="B139" s="51" t="s">
+      <c r="A139" s="60"/>
+      <c r="B139" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C139" s="34"/>
-      <c r="D139" s="34"/>
-      <c r="E139" s="34"/>
+      <c r="C139" s="33"/>
+      <c r="D139" s="33"/>
+      <c r="E139" s="33"/>
     </row>
     <row r="140" spans="1:5" ht="15" customHeight="1">
-      <c r="A140" s="55" t="s">
+      <c r="A140" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B140" s="51" t="s">
+      <c r="B140" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C140" s="34"/>
-      <c r="D140" s="34"/>
-      <c r="E140" s="34"/>
+      <c r="C140" s="33"/>
+      <c r="D140" s="33"/>
+      <c r="E140" s="33"/>
     </row>
     <row r="141" spans="1:5" ht="15" customHeight="1">
-      <c r="A141" s="53"/>
-      <c r="B141" s="51"/>
-      <c r="C141" s="34"/>
-      <c r="D141" s="34"/>
-      <c r="E141" s="34"/>
+      <c r="A141" s="59"/>
+      <c r="B141" s="57"/>
+      <c r="C141" s="33"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="33"/>
     </row>
     <row r="142" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A142" s="54"/>
-      <c r="B142" s="51"/>
-      <c r="C142" s="34"/>
-      <c r="D142" s="34"/>
-      <c r="E142" s="34"/>
+      <c r="A142" s="60"/>
+      <c r="B142" s="57"/>
+      <c r="C142" s="33"/>
+      <c r="D142" s="33"/>
+      <c r="E142" s="33"/>
     </row>
     <row r="143" spans="1:5" ht="15" customHeight="1">
-      <c r="A143" s="49" t="s">
+      <c r="A143" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B143" s="51" t="s">
+      <c r="B143" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C143" s="34"/>
-      <c r="D143" s="34"/>
-      <c r="E143" s="34"/>
+      <c r="C143" s="33"/>
+      <c r="D143" s="33"/>
+      <c r="E143" s="33"/>
     </row>
     <row r="144" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A144" s="50"/>
-      <c r="B144" s="51" t="s">
+      <c r="A144" s="56"/>
+      <c r="B144" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C144" s="34"/>
-      <c r="D144" s="34"/>
-      <c r="E144" s="34"/>
+      <c r="C144" s="33"/>
+      <c r="D144" s="33"/>
+      <c r="E144" s="33"/>
     </row>
     <row r="145" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A145" s="59"/>
+      <c r="A145" s="67"/>
       <c r="B145" s="11"/>
       <c r="C145" s="12"/>
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
     </row>
     <row r="146" spans="1:6" ht="15" customHeight="1">
-      <c r="A146" s="49" t="s">
+      <c r="A146" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B146" s="51" t="s">
+      <c r="B146" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C146" s="34"/>
-      <c r="D146" s="34"/>
-      <c r="E146" s="34"/>
+      <c r="C146" s="33"/>
+      <c r="D146" s="33"/>
+      <c r="E146" s="33"/>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="50"/>
-      <c r="B147" s="51"/>
-      <c r="C147" s="34"/>
-      <c r="D147" s="34"/>
-      <c r="E147" s="34"/>
+      <c r="A147" s="56"/>
+      <c r="B147" s="57"/>
+      <c r="C147" s="33"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="33"/>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B149" s="62" t="s">
+      <c r="B149" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C149" s="62"/>
-      <c r="D149" s="62"/>
-      <c r="E149" s="62"/>
+      <c r="C149" s="52"/>
+      <c r="D149" s="52"/>
+      <c r="E149" s="52"/>
     </row>
     <row r="150" spans="1:6">
-      <c r="A150" s="63" t="s">
+      <c r="A150" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B150" s="64" t="s">
+      <c r="B150" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C150" s="64"/>
-      <c r="D150" s="64"/>
-      <c r="E150" s="64"/>
+      <c r="C150" s="54"/>
+      <c r="D150" s="54"/>
+      <c r="E150" s="54"/>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="63"/>
-      <c r="B151" s="64"/>
-      <c r="C151" s="64"/>
-      <c r="D151" s="64"/>
-      <c r="E151" s="64"/>
+      <c r="A151" s="53"/>
+      <c r="B151" s="54"/>
+      <c r="C151" s="54"/>
+      <c r="D151" s="54"/>
+      <c r="E151" s="54"/>
     </row>
     <row r="154" spans="1:6" ht="21">
       <c r="A154" s="13" t="s">
@@ -3327,13 +3305,13 @@
     </row>
     <row r="158" spans="1:6" ht="15.75" thickBot="1">
       <c r="A158" s="9"/>
-      <c r="B158" s="60" t="s">
+      <c r="B158" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C158" s="60"/>
-      <c r="D158" s="60"/>
-      <c r="E158" s="60"/>
-      <c r="F158" s="61"/>
+      <c r="C158" s="61"/>
+      <c r="D158" s="61"/>
+      <c r="E158" s="61"/>
+      <c r="F158" s="62"/>
     </row>
     <row r="159" spans="1:6" ht="15.75" thickBot="1">
       <c r="A159" s="7" t="s">
@@ -3585,183 +3563,247 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A173" s="58" t="s">
+      <c r="A173" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B173" s="58"/>
-      <c r="C173" s="58"/>
-      <c r="D173" s="58"/>
-      <c r="E173" s="58"/>
+      <c r="B173" s="63"/>
+      <c r="C173" s="63"/>
+      <c r="D173" s="63"/>
+      <c r="E173" s="63"/>
     </row>
     <row r="174" spans="1:6" ht="15.75" thickBot="1">
       <c r="A174" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B174" s="56" t="s">
+      <c r="B174" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C174" s="57"/>
-      <c r="D174" s="57"/>
-      <c r="E174" s="57"/>
+      <c r="C174" s="65"/>
+      <c r="D174" s="65"/>
+      <c r="E174" s="65"/>
     </row>
     <row r="175" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A175" s="52" t="s">
+      <c r="A175" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B175" s="51" t="s">
+      <c r="B175" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C175" s="34"/>
-      <c r="D175" s="34"/>
-      <c r="E175" s="34"/>
+      <c r="C175" s="33"/>
+      <c r="D175" s="33"/>
+      <c r="E175" s="33"/>
     </row>
     <row r="176" spans="1:6" ht="15" customHeight="1">
-      <c r="A176" s="53"/>
-      <c r="B176" s="51" t="s">
+      <c r="A176" s="59"/>
+      <c r="B176" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C176" s="34"/>
-      <c r="D176" s="34"/>
-      <c r="E176" s="34"/>
+      <c r="C176" s="33"/>
+      <c r="D176" s="33"/>
+      <c r="E176" s="33"/>
     </row>
     <row r="177" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A177" s="54"/>
-      <c r="B177" s="51"/>
-      <c r="C177" s="34"/>
-      <c r="D177" s="34"/>
-      <c r="E177" s="34"/>
+      <c r="A177" s="60"/>
+      <c r="B177" s="57"/>
+      <c r="C177" s="33"/>
+      <c r="D177" s="33"/>
+      <c r="E177" s="33"/>
     </row>
     <row r="178" spans="1:5" ht="15" customHeight="1">
-      <c r="A178" s="55" t="s">
+      <c r="A178" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B178" s="51" t="s">
+      <c r="B178" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C178" s="34"/>
-      <c r="D178" s="34"/>
-      <c r="E178" s="34"/>
+      <c r="C178" s="33"/>
+      <c r="D178" s="33"/>
+      <c r="E178" s="33"/>
     </row>
     <row r="179" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A179" s="54"/>
-      <c r="B179" s="51"/>
-      <c r="C179" s="34"/>
-      <c r="D179" s="34"/>
-      <c r="E179" s="34"/>
+      <c r="A179" s="60"/>
+      <c r="B179" s="57"/>
+      <c r="C179" s="33"/>
+      <c r="D179" s="33"/>
+      <c r="E179" s="33"/>
     </row>
     <row r="180" spans="1:5" ht="15" customHeight="1">
-      <c r="A180" s="55" t="s">
+      <c r="A180" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B180" s="51" t="s">
+      <c r="B180" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C180" s="34"/>
-      <c r="D180" s="34"/>
-      <c r="E180" s="34"/>
+      <c r="C180" s="33"/>
+      <c r="D180" s="33"/>
+      <c r="E180" s="33"/>
     </row>
     <row r="181" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A181" s="54"/>
-      <c r="B181" s="51"/>
-      <c r="C181" s="34"/>
-      <c r="D181" s="34"/>
-      <c r="E181" s="34"/>
+      <c r="A181" s="60"/>
+      <c r="B181" s="57"/>
+      <c r="C181" s="33"/>
+      <c r="D181" s="33"/>
+      <c r="E181" s="33"/>
     </row>
     <row r="182" spans="1:5" ht="15" customHeight="1">
-      <c r="A182" s="55" t="s">
+      <c r="A182" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B182" s="51" t="s">
+      <c r="B182" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C182" s="34"/>
-      <c r="D182" s="34"/>
-      <c r="E182" s="34"/>
+      <c r="C182" s="33"/>
+      <c r="D182" s="33"/>
+      <c r="E182" s="33"/>
     </row>
     <row r="183" spans="1:5" ht="15" customHeight="1">
-      <c r="A183" s="53"/>
-      <c r="B183" s="51" t="s">
+      <c r="A183" s="59"/>
+      <c r="B183" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C183" s="34"/>
-      <c r="D183" s="34"/>
-      <c r="E183" s="34"/>
+      <c r="C183" s="33"/>
+      <c r="D183" s="33"/>
+      <c r="E183" s="33"/>
     </row>
     <row r="184" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A184" s="54"/>
-      <c r="B184" s="51" t="s">
+      <c r="A184" s="60"/>
+      <c r="B184" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C184" s="34"/>
-      <c r="D184" s="34"/>
-      <c r="E184" s="34"/>
+      <c r="C184" s="33"/>
+      <c r="D184" s="33"/>
+      <c r="E184" s="33"/>
     </row>
     <row r="185" spans="1:5" ht="15" customHeight="1">
-      <c r="A185" s="55" t="s">
+      <c r="A185" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B185" s="51" t="s">
+      <c r="B185" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C185" s="34"/>
-      <c r="D185" s="34"/>
-      <c r="E185" s="34"/>
+      <c r="C185" s="33"/>
+      <c r="D185" s="33"/>
+      <c r="E185" s="33"/>
     </row>
     <row r="186" spans="1:5">
-      <c r="A186" s="53"/>
-      <c r="B186" s="51"/>
-      <c r="C186" s="34"/>
-      <c r="D186" s="34"/>
-      <c r="E186" s="34"/>
+      <c r="A186" s="59"/>
+      <c r="B186" s="57"/>
+      <c r="C186" s="33"/>
+      <c r="D186" s="33"/>
+      <c r="E186" s="33"/>
     </row>
     <row r="187" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A187" s="54"/>
-      <c r="B187" s="51"/>
-      <c r="C187" s="34"/>
-      <c r="D187" s="34"/>
-      <c r="E187" s="34"/>
+      <c r="A187" s="60"/>
+      <c r="B187" s="57"/>
+      <c r="C187" s="33"/>
+      <c r="D187" s="33"/>
+      <c r="E187" s="33"/>
     </row>
     <row r="188" spans="1:5" ht="15" customHeight="1">
-      <c r="A188" s="49" t="s">
+      <c r="A188" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="51" t="s">
+      <c r="B188" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C188" s="34"/>
-      <c r="D188" s="34"/>
-      <c r="E188" s="34"/>
+      <c r="C188" s="33"/>
+      <c r="D188" s="33"/>
+      <c r="E188" s="33"/>
     </row>
     <row r="189" spans="1:5" ht="15" customHeight="1">
-      <c r="A189" s="50"/>
-      <c r="B189" s="51" t="s">
+      <c r="A189" s="56"/>
+      <c r="B189" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C189" s="34"/>
-      <c r="D189" s="34"/>
-      <c r="E189" s="34"/>
+      <c r="C189" s="33"/>
+      <c r="D189" s="33"/>
+      <c r="E189" s="33"/>
     </row>
     <row r="190" spans="1:5">
-      <c r="A190" s="50"/>
+      <c r="A190" s="56"/>
       <c r="B190" s="18"/>
       <c r="C190" s="19"/>
       <c r="D190" s="19"/>
       <c r="E190" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="112">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
+  <mergeCells count="110">
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B129:E129"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="B132:E132"/>
+    <mergeCell ref="A128:E128"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B134:E134"/>
+    <mergeCell ref="B135:E135"/>
+    <mergeCell ref="B136:E136"/>
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:E175"/>
+    <mergeCell ref="B176:E176"/>
+    <mergeCell ref="B177:E177"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B140:E140"/>
+    <mergeCell ref="B142:E142"/>
+    <mergeCell ref="B143:E143"/>
+    <mergeCell ref="B144:E144"/>
+    <mergeCell ref="B138:E138"/>
+    <mergeCell ref="A137:A139"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="B139:E139"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:E146"/>
+    <mergeCell ref="B147:E147"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:E151"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="B188:E188"/>
+    <mergeCell ref="B189:E189"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="B183:E183"/>
+    <mergeCell ref="B184:E184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="B185:E185"/>
+    <mergeCell ref="B186:E186"/>
+    <mergeCell ref="B187:E187"/>
+    <mergeCell ref="A178:A179"/>
+    <mergeCell ref="B178:E178"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="B180:E180"/>
+    <mergeCell ref="B181:E181"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="B174:E174"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="B21:E21"/>
@@ -3786,82 +3828,16 @@
     <mergeCell ref="A92:A94"/>
     <mergeCell ref="B92:E92"/>
     <mergeCell ref="B93:E93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:E151"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="B188:E188"/>
-    <mergeCell ref="B189:E189"/>
-    <mergeCell ref="A182:A184"/>
-    <mergeCell ref="B182:E182"/>
-    <mergeCell ref="B183:E183"/>
-    <mergeCell ref="B184:E184"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="B185:E185"/>
-    <mergeCell ref="B186:E186"/>
-    <mergeCell ref="B187:E187"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="B178:E178"/>
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="B180:E180"/>
-    <mergeCell ref="B181:E181"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="B174:E174"/>
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:E175"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="B177:E177"/>
-    <mergeCell ref="B137:E137"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B140:E140"/>
-    <mergeCell ref="B142:E142"/>
-    <mergeCell ref="B143:E143"/>
-    <mergeCell ref="B144:E144"/>
-    <mergeCell ref="B138:E138"/>
-    <mergeCell ref="A137:A139"/>
-    <mergeCell ref="A140:A142"/>
-    <mergeCell ref="B139:E139"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:E146"/>
-    <mergeCell ref="B147:E147"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B129:E129"/>
-    <mergeCell ref="B130:E130"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="B132:E132"/>
-    <mergeCell ref="A128:E128"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B134:E134"/>
-    <mergeCell ref="B135:E135"/>
-    <mergeCell ref="B136:E136"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>